<commit_message>
Contact info changed in test case 520
</commit_message>
<xml_diff>
--- a/test_files/Code_list_with_feedback_column.xlsx
+++ b/test_files/Code_list_with_feedback_column.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22119"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E1FE8BF2-FF75-47C2-BDF9-668138B07BB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{31F9386A-7098-437B-B1D1-D7B21340913C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12,14 +12,6 @@
     <sheet name="Codes" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -143,13 +135,13 @@
     <t>sitovuustasoFI</t>
   </si>
   <si>
-    <t>Yläpitäjän yhteystiedot_fi</t>
-  </si>
-  <si>
-    <t>Yläpitäjän yhteystiedot_en</t>
-  </si>
-  <si>
-    <t>Ylläpitäjän yhteystiedot_sw-UG</t>
+    <t>Aineiston palauteosoite_fi</t>
+  </si>
+  <si>
+    <t>Aineiston palauteosoite_en</t>
+  </si>
+  <si>
+    <t>Aineiston palauteosoite_sw-UG</t>
   </si>
   <si>
     <t>fi;en;sw-UG</t>
@@ -604,8 +596,8 @@
   </sheetPr>
   <dimension ref="A1:AA1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="X2" sqref="X2"/>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="Z2" sqref="Z2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>